<commit_message>
[New] - 備份20240408資料 [Revise] - 修改TableSchema
</commit_message>
<xml_diff>
--- a/Schema/TableSchema.xlsx
+++ b/Schema/TableSchema.xlsx
@@ -14,7 +14,9 @@
   <sheets>
     <sheet name="Member_Schema" sheetId="2" r:id="rId1"/>
     <sheet name="MessageBoard_Schema" sheetId="4" r:id="rId2"/>
-    <sheet name="ErrorLog_Schema" sheetId="1" r:id="rId3"/>
+    <sheet name="PictureTable_Schema" sheetId="6" r:id="rId3"/>
+    <sheet name="ErrorLog_Schema" sheetId="1" r:id="rId4"/>
+    <sheet name="Cache_Schema" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="69">
   <si>
     <t>項目序號</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -245,6 +247,62 @@
   </si>
   <si>
     <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ExpiresAtTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SlidingExpirationInSeconds</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AbsoluteExpiration</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varbinary</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>datetimeoffset</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bigint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PictureId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PictureName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CreateTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>建立時間</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>圖片名稱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>圖片編號</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -312,7 +370,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -455,13 +513,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -530,6 +627,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -836,10 +948,10 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22"/>
+      <c r="D1" s="23"/>
       <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1054,10 +1166,10 @@
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22"/>
+      <c r="D1" s="23"/>
       <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
@@ -1219,6 +1331,197 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="23"/>
+      <c r="E1" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="20">
+        <v>1</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="9"/>
+      <c r="I3" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="20">
+        <v>2</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="9"/>
+      <c r="I4" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="20">
+        <v>3</v>
+      </c>
+      <c r="B5" s="14"/>
+      <c r="C5" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="14">
+        <v>10</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="I5" s="10"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="20">
+        <v>4</v>
+      </c>
+      <c r="B6" s="14"/>
+      <c r="C6" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="9"/>
+      <c r="I6" s="10"/>
+    </row>
+    <row r="7" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="11"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:D1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="257" orientation="portrait" horizontalDpi="204" verticalDpi="196" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
@@ -1245,10 +1548,10 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22"/>
+      <c r="D1" s="23"/>
       <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1405,4 +1708,205 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="257" orientation="portrait" horizontalDpi="204" verticalDpi="196" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="23"/>
+      <c r="E1" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="20">
+        <v>1</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="14">
+        <v>449</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="9"/>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="20">
+        <v>2</v>
+      </c>
+      <c r="B4" s="14"/>
+      <c r="C4" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="9"/>
+      <c r="I4" s="10"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="20">
+        <v>3</v>
+      </c>
+      <c r="B5" s="14"/>
+      <c r="C5" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="14">
+        <v>7</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="I5" s="10"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="20">
+        <v>4</v>
+      </c>
+      <c r="B6" s="14"/>
+      <c r="C6" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" s="9"/>
+      <c r="I6" s="10"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="24">
+        <v>5</v>
+      </c>
+      <c r="B7" s="25"/>
+      <c r="C7" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="26"/>
+      <c r="E7" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="25">
+        <v>7</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="26"/>
+      <c r="I7" s="27"/>
+    </row>
+    <row r="8" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="11"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:D1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="257" orientation="portrait" horizontalDpi="204" verticalDpi="196" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>